<commit_message>
feat(schedule): use driver buckets for planning
</commit_message>
<xml_diff>
--- a/testFiles/followupBy test.xlsx
+++ b/testFiles/followupBy test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6718527680502480/Coding/ICjourney/testFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7" documentId="8_{9E3A5FF0-E345-48E3-8D9C-BD236BB297BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C67D9FC0-8769-4137-94F8-74BA1ECB87D3}"/>
+  <xr:revisionPtr revIDLastSave="24" documentId="8_{9E3A5FF0-E345-48E3-8D9C-BD236BB297BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4D7EB04D-BA8C-4385-9C2A-40135796F0B0}"/>
   <bookViews>
-    <workbookView xWindow="33105" yWindow="-2190" windowWidth="27390" windowHeight="19200" xr2:uid="{ED27B8AF-98B3-463E-83B7-9FB6BD236B8B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{ED27B8AF-98B3-463E-83B7-9FB6BD236B8B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25519,6 +25519,10 @@
 </externalLink>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -25838,11 +25842,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B606923F-9EE5-4858-8140-D7EDCB240659}">
   <dimension ref="A1:L18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:L18"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="7" max="7" width="9.42578125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="27" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
@@ -25902,9 +25909,8 @@
         <f>IFERROR(VLOOKUP(B2, [1]Visited!$B$2:$C$743, 2, FALSE), "")</f>
         <v>6/28/2024 1:29:16 PM</v>
       </c>
-      <c r="G2" s="11" t="str">
-        <f>TEXT(F2, "mm-dd-yyyy")</f>
-        <v>06-28-2024</v>
+      <c r="G2" s="13">
+        <v>46174</v>
       </c>
       <c r="H2" s="14" t="str">
         <f>IFERROR(VLOOKUP(B2, [1]Volume!$B$2:$C$1000, 2, FALSE), "")</f>
@@ -25947,9 +25953,8 @@
         <f>IFERROR(VLOOKUP(B3, [1]Visited!$B$2:$C$743, 2, FALSE), "")</f>
         <v>45334.568773148145</v>
       </c>
-      <c r="G3" s="11" t="str">
-        <f t="shared" ref="G3" si="0">TEXT(F3, "mm-dd-yyyy")</f>
-        <v>02-12-2024</v>
+      <c r="G3" s="13">
+        <v>46174</v>
       </c>
       <c r="H3" s="14">
         <f>IFERROR(VLOOKUP(B3, [1]Volume!$B$2:$C$1000, 2, FALSE), "")</f>
@@ -25992,9 +25997,8 @@
         <f>IFERROR(VLOOKUP(B4, [1]Visited!$B$2:$C$743, 2, FALSE), "")</f>
         <v>1/8/2025 9:17:07 AM</v>
       </c>
-      <c r="G4" s="11" t="str">
-        <f>TEXT(F4, "mm-dd-yyyy")</f>
-        <v>01-08-2025</v>
+      <c r="G4" s="13">
+        <v>46174</v>
       </c>
       <c r="H4" s="14" t="str">
         <f>IFERROR(VLOOKUP(B4, [1]Volume!$B$2:$C$1000, 2, FALSE), "")</f>
@@ -26038,9 +26042,8 @@
         <f>IFERROR(VLOOKUP(B5, [1]Visited!$B$2:$C$743, 2, FALSE), "")</f>
         <v>8/30/2024 9:59:39 AM</v>
       </c>
-      <c r="G5" s="11" t="str">
-        <f>TEXT(F5, "mm-dd-yyyy")</f>
-        <v>08-30-2024</v>
+      <c r="G5" s="13">
+        <v>46027</v>
       </c>
       <c r="H5" s="14">
         <f>IFERROR(VLOOKUP(B5, [1]Volume!$B$2:$C$1000, 2, FALSE), "")</f>
@@ -26083,9 +26086,8 @@
         <f>IFERROR(VLOOKUP(B6, [1]Visited!$B$2:$C$743, 2, FALSE), "")</f>
         <v>12/30/2024 2:00:56 PM</v>
       </c>
-      <c r="G6" s="11" t="str">
-        <f>TEXT(F6, "mm-dd-yyyy")</f>
-        <v>12-30-2024</v>
+      <c r="G6" s="13">
+        <v>46174</v>
       </c>
       <c r="H6" s="14">
         <f>IFERROR(VLOOKUP(B6, [1]Volume!$B$2:$C$1000, 2, FALSE), "")</f>
@@ -26128,9 +26130,8 @@
         <f>IFERROR(VLOOKUP(B7, [1]Visited!$B$2:$C$743, 2, FALSE), "")</f>
         <v>1/28/2025 12:45:54 PM</v>
       </c>
-      <c r="G7" s="11" t="str">
-        <f>TEXT(F7, "mm-dd-yyyy")</f>
-        <v>01-28-2025</v>
+      <c r="G7" s="13">
+        <v>46204</v>
       </c>
       <c r="H7" s="14" t="str">
         <f>IFERROR(VLOOKUP(B7, [1]Volume!$B$2:$C$1000, 2, FALSE), "")</f>
@@ -26172,9 +26173,8 @@
         <f>IFERROR(VLOOKUP(B8, [1]Visited!$B$2:$C$743, 2, FALSE), "")</f>
         <v>1/28/2025 12:45:54 PM</v>
       </c>
-      <c r="G8" s="11" t="str">
-        <f>TEXT(F8, "mm-dd-yyyy")</f>
-        <v>01-28-2025</v>
+      <c r="G8" s="13">
+        <v>46027</v>
       </c>
       <c r="H8" s="14" t="str">
         <f>IFERROR(VLOOKUP(B8, [1]Volume!$B$2:$C$1000, 2, FALSE), "")</f>
@@ -26215,9 +26215,8 @@
         <f>IFERROR(VLOOKUP(B9, [1]Visited!$B$2:$C$743, 2, FALSE), "")</f>
         <v>12/13/2024 12:45:59 PM</v>
       </c>
-      <c r="G9" s="11" t="str">
-        <f>TEXT(F9, "mm-dd-yyyy")</f>
-        <v>12-13-2024</v>
+      <c r="G9" s="13">
+        <v>46204</v>
       </c>
       <c r="H9" s="14" t="str">
         <f>IFERROR(VLOOKUP(B9, [1]Volume!$B$2:$C$1000, 2, FALSE), "")</f>
@@ -26260,9 +26259,8 @@
         <f>IFERROR(VLOOKUP(B10, [1]Visited!$B$2:$C$743, 2, FALSE), "")</f>
         <v>1/23/2025 12:21:31 PM</v>
       </c>
-      <c r="G10" s="11" t="str">
-        <f>TEXT(F10, "mm-dd-yyyy")</f>
-        <v>01-23-2025</v>
+      <c r="G10" s="13">
+        <v>46174</v>
       </c>
       <c r="H10" s="14" t="str">
         <f>IFERROR(VLOOKUP(B10, [1]Volume!$B$2:$C$1000, 2, FALSE), "")</f>
@@ -26307,9 +26305,8 @@
         <f>IFERROR(VLOOKUP(B11, [1]Visited!$B$2:$C$743, 2, FALSE), "")</f>
         <v>11/14/2024 2:50:59 PM</v>
       </c>
-      <c r="G11" s="11" t="str">
-        <f>TEXT(F11, "mm-dd-yyyy")</f>
-        <v>11-14-2024</v>
+      <c r="G11" s="13">
+        <v>46204</v>
       </c>
       <c r="H11" s="14" t="str">
         <f>IFERROR(VLOOKUP(B11, [1]Volume!$B$2:$C$1000, 2, FALSE), "")</f>
@@ -26352,9 +26349,8 @@
         <f>IFERROR(VLOOKUP(B12, [1]Visited!$B$2:$C$743, 2, FALSE), "")</f>
         <v>11/25/2024 5:06:26 PM</v>
       </c>
-      <c r="G12" s="11" t="str">
-        <f>TEXT(F12, "mm-dd-yyyy")</f>
-        <v>11-25-2024</v>
+      <c r="G12" s="13">
+        <v>46025</v>
       </c>
       <c r="H12" s="14">
         <f>IFERROR(VLOOKUP(B12, [1]Volume!$B$2:$C$1000, 2, FALSE), "")</f>
@@ -26397,9 +26393,8 @@
         <f>IFERROR(VLOOKUP(B13, [1]Visited!$B$2:$C$743, 2, FALSE), "")</f>
         <v>45484.545081018521</v>
       </c>
-      <c r="G13" s="11" t="str">
-        <f>TEXT(F13, "mm-dd-yyyy")</f>
-        <v>07-11-2024</v>
+      <c r="G13" s="13">
+        <v>46025</v>
       </c>
       <c r="H13" s="14">
         <f>IFERROR(VLOOKUP(B13, [1]Volume!$B$2:$C$1000, 2, FALSE), "")</f>
@@ -26442,9 +26437,8 @@
         <f>IFERROR(VLOOKUP(B14, [1]Visited!$B$2:$C$743, 2, FALSE), "")</f>
         <v>1/22/2025 10:36:37 AM</v>
       </c>
-      <c r="G14" s="11" t="str">
-        <f>TEXT(F14, "mm-dd-yyyy")</f>
-        <v>01-22-2025</v>
+      <c r="G14" s="13">
+        <v>46025</v>
       </c>
       <c r="H14" s="14" t="str">
         <f>IFERROR(VLOOKUP(B14, [1]Volume!$B$2:$C$1000, 2, FALSE), "")</f>
@@ -26488,9 +26482,8 @@
         <f>IFERROR(VLOOKUP(B15, [1]Visited!$B$2:$C$743, 2, FALSE), "")</f>
         <v>45484.573587962965</v>
       </c>
-      <c r="G15" s="11" t="str">
-        <f>TEXT(F15, "mm-dd-yyyy")</f>
-        <v>07-11-2024</v>
+      <c r="G15" s="13">
+        <v>46296</v>
       </c>
       <c r="H15" s="14">
         <f>IFERROR(VLOOKUP(B15, [1]Volume!$B$2:$C$1000, 2, FALSE), "")</f>
@@ -26533,9 +26526,8 @@
         <f>IFERROR(VLOOKUP(B16, [1]Visited!$B$2:$C$743, 2, FALSE), "")</f>
         <v>1/10/2025 12:23:53 PM</v>
       </c>
-      <c r="G16" s="11" t="str">
-        <f>TEXT(F16, "mm-dd-yyyy")</f>
-        <v>01-10-2025</v>
+      <c r="G16" s="13">
+        <v>46027</v>
       </c>
       <c r="H16" s="14" t="str">
         <f>IFERROR(VLOOKUP(B16, [1]Volume!$B$2:$C$1000, 2, FALSE), "")</f>
@@ -26579,9 +26571,8 @@
         <f>IFERROR(VLOOKUP(B17, [1]Visited!$B$2:$C$743, 2, FALSE), "")</f>
         <v>45569.571296296293</v>
       </c>
-      <c r="G17" s="11" t="str">
-        <f>TEXT(F17, "mm-dd-yyyy")</f>
-        <v>10-04-2024</v>
+      <c r="G17" s="13">
+        <v>46296</v>
       </c>
       <c r="H17" s="14" t="str">
         <f>IFERROR(VLOOKUP(B17, [1]Volume!$B$2:$C$1000, 2, FALSE), "")</f>
@@ -26624,9 +26615,8 @@
         <f>IFERROR(VLOOKUP(B18, [1]Visited!$B$2:$C$743, 2, FALSE), "")</f>
         <v>1/15/2025 12:04:33 PM</v>
       </c>
-      <c r="G18" s="11" t="str">
-        <f>TEXT(F18, "mm-dd-yyyy")</f>
-        <v>01-15-2025</v>
+      <c r="G18" s="13">
+        <v>46027</v>
       </c>
       <c r="H18" s="14" t="str">
         <f>IFERROR(VLOOKUP(B18, [1]Volume!$B$2:$C$1000, 2, FALSE), "")</f>

</xml_diff>

<commit_message>
fix(schedule): apply effective drivers and list sources
</commit_message>
<xml_diff>
--- a/testFiles/followupBy test.xlsx
+++ b/testFiles/followupBy test.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -25842,7 +25842,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B606923F-9EE5-4858-8140-D7EDCB240659}">
   <dimension ref="A1:L18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
chore: keep local updates and test files
</commit_message>
<xml_diff>
--- a/testFiles/followupBy test.xlsx
+++ b/testFiles/followupBy test.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="24" documentId="8_{9E3A5FF0-E345-48E3-8D9C-BD236BB297BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4D7EB04D-BA8C-4385-9C2A-40135796F0B0}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{ED27B8AF-98B3-463E-83B7-9FB6BD236B8B}"/>
+    <workbookView xWindow="375" yWindow="150" windowWidth="13350" windowHeight="14325" xr2:uid="{ED27B8AF-98B3-463E-83B7-9FB6BD236B8B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25842,8 +25842,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B606923F-9EE5-4858-8140-D7EDCB240659}">
   <dimension ref="A1:L18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Add audit dates script and config
</commit_message>
<xml_diff>
--- a/testFiles/followupBy test.xlsx
+++ b/testFiles/followupBy test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6718527680502480/Coding/ICjourney/testFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="24" documentId="8_{9E3A5FF0-E345-48E3-8D9C-BD236BB297BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4D7EB04D-BA8C-4385-9C2A-40135796F0B0}"/>
+  <xr:revisionPtr revIDLastSave="25" documentId="8_{9E3A5FF0-E345-48E3-8D9C-BD236BB297BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D9A04F96-3A64-48E6-89D1-E56CE6F73431}"/>
   <bookViews>
-    <workbookView xWindow="375" yWindow="150" windowWidth="13350" windowHeight="14325" xr2:uid="{ED27B8AF-98B3-463E-83B7-9FB6BD236B8B}"/>
+    <workbookView xWindow="35730" yWindow="-210" windowWidth="21975" windowHeight="10905" xr2:uid="{ED27B8AF-98B3-463E-83B7-9FB6BD236B8B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -66,9 +66,6 @@
   </si>
   <si>
     <t>rm</t>
-  </si>
-  <si>
-    <t>last_visited2.0</t>
   </si>
   <si>
     <t>top_volume</t>
@@ -231,6 +228,9 @@
   </si>
   <si>
     <t>CO1 1DN</t>
+  </si>
+  <si>
+    <t>2.0 last_visit</t>
   </si>
 </sst>
 </file>
@@ -25842,8 +25842,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B606923F-9EE5-4858-8140-D7EDCB240659}">
   <dimension ref="A1:L18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -25868,42 +25868,42 @@
         <v>8</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>9</v>
+        <v>63</v>
       </c>
       <c r="G1" s="6" t="s">
         <v>3</v>
       </c>
       <c r="H1" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="J1" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="J1" s="8" t="s">
+      <c r="K1" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="K1" s="8" t="s">
+      <c r="L1" s="6" t="s">
         <v>13</v>
-      </c>
-      <c r="L1" s="6" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="105" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="C2" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="D2" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="E2" s="12" t="s">
         <v>18</v>
-      </c>
-      <c r="E2" s="12" t="s">
-        <v>19</v>
       </c>
       <c r="F2" s="13" t="str">
         <f>IFERROR(VLOOKUP(B2, [1]Visited!$B$2:$C$743, 2, FALSE), "")</f>
@@ -25935,19 +25935,19 @@
     </row>
     <row r="3" spans="1:12" ht="90" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="C3" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" s="11" t="s">
+      <c r="E3" s="12" t="s">
         <v>22</v>
-      </c>
-      <c r="E3" s="12" t="s">
-        <v>23</v>
       </c>
       <c r="F3" s="13">
         <f>IFERROR(VLOOKUP(B3, [1]Visited!$B$2:$C$743, 2, FALSE), "")</f>
@@ -25979,19 +25979,19 @@
     </row>
     <row r="4" spans="1:12" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="C4" s="10" t="s">
         <v>25</v>
-      </c>
-      <c r="C4" s="10" t="s">
-        <v>26</v>
       </c>
       <c r="D4" s="11" t="s">
         <v>5</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F4" s="13" t="str">
         <f>IFERROR(VLOOKUP(B4, [1]Visited!$B$2:$C$743, 2, FALSE), "")</f>
@@ -26024,19 +26024,19 @@
     </row>
     <row r="5" spans="1:12" ht="150" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C5" s="10" t="s">
         <v>6</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F5" s="13" t="str">
         <f>IFERROR(VLOOKUP(B5, [1]Visited!$B$2:$C$743, 2, FALSE), "")</f>
@@ -26068,19 +26068,19 @@
     </row>
     <row r="6" spans="1:12" ht="75" x14ac:dyDescent="0.25">
       <c r="A6" s="17" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C6" s="14" t="s">
         <v>6</v>
       </c>
       <c r="D6" s="15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E6" s="18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F6" s="13" t="str">
         <f>IFERROR(VLOOKUP(B6, [1]Visited!$B$2:$C$743, 2, FALSE), "")</f>
@@ -26112,19 +26112,19 @@
     </row>
     <row r="7" spans="1:12" ht="165" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="B7" s="10" t="s">
-        <v>36</v>
-      </c>
       <c r="C7" s="10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F7" s="13" t="str">
         <f>IFERROR(VLOOKUP(B7, [1]Visited!$B$2:$C$743, 2, FALSE), "")</f>
@@ -26157,13 +26157,13 @@
     </row>
     <row r="8" spans="1:12" ht="165" x14ac:dyDescent="0.25">
       <c r="A8" s="19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D8" s="11" t="s">
         <v>5</v>
@@ -26197,19 +26197,19 @@
     </row>
     <row r="9" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A9" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="B9" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="B9" s="14" t="s">
-        <v>40</v>
-      </c>
       <c r="C9" s="14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D9" s="15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E9" s="15" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F9" s="13" t="str">
         <f>IFERROR(VLOOKUP(B9, [1]Visited!$B$2:$C$743, 2, FALSE), "")</f>
@@ -26241,7 +26241,7 @@
     </row>
     <row r="10" spans="1:12" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B10" s="10" t="s">
         <v>4</v>
@@ -26250,10 +26250,10 @@
         <v>6</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F10" s="13" t="str">
         <f>IFERROR(VLOOKUP(B10, [1]Visited!$B$2:$C$743, 2, FALSE), "")</f>
@@ -26287,19 +26287,19 @@
     </row>
     <row r="11" spans="1:12" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A11" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="B11" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="B11" s="14" t="s">
-        <v>44</v>
-      </c>
       <c r="C11" s="14" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D11" s="15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E11" s="18" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F11" s="13" t="str">
         <f>IFERROR(VLOOKUP(B11, [1]Visited!$B$2:$C$743, 2, FALSE), "")</f>
@@ -26331,19 +26331,19 @@
     </row>
     <row r="12" spans="1:12" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A12" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="B12" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="B12" s="14" t="s">
-        <v>47</v>
-      </c>
       <c r="C12" s="14" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D12" s="15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E12" s="18" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F12" s="13" t="str">
         <f>IFERROR(VLOOKUP(B12, [1]Visited!$B$2:$C$743, 2, FALSE), "")</f>
@@ -26375,19 +26375,19 @@
     </row>
     <row r="13" spans="1:12" ht="150" x14ac:dyDescent="0.25">
       <c r="A13" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="B13" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="B13" s="15" t="s">
-        <v>50</v>
-      </c>
       <c r="C13" s="15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D13" s="15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E13" s="18" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F13" s="13">
         <f>IFERROR(VLOOKUP(B13, [1]Visited!$B$2:$C$743, 2, FALSE), "")</f>
@@ -26419,19 +26419,19 @@
     </row>
     <row r="14" spans="1:12" ht="285" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="B14" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="B14" s="10" t="s">
-        <v>53</v>
-      </c>
       <c r="C14" s="10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D14" s="11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E14" s="12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F14" s="13" t="str">
         <f>IFERROR(VLOOKUP(B14, [1]Visited!$B$2:$C$743, 2, FALSE), "")</f>
@@ -26464,19 +26464,19 @@
     </row>
     <row r="15" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A15" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="B15" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="B15" s="15" t="s">
-        <v>55</v>
-      </c>
       <c r="C15" s="15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D15" s="15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E15" s="18" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F15" s="13">
         <f>IFERROR(VLOOKUP(B15, [1]Visited!$B$2:$C$743, 2, FALSE), "")</f>
@@ -26508,19 +26508,19 @@
     </row>
     <row r="16" spans="1:12" ht="195" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="B16" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="B16" s="10" t="s">
-        <v>57</v>
-      </c>
       <c r="C16" s="10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D16" s="11" t="s">
         <v>5</v>
       </c>
       <c r="E16" s="12" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F16" s="13" t="str">
         <f>IFERROR(VLOOKUP(B16, [1]Visited!$B$2:$C$743, 2, FALSE), "")</f>
@@ -26553,19 +26553,19 @@
     </row>
     <row r="17" spans="1:12" ht="90" x14ac:dyDescent="0.25">
       <c r="A17" s="20" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B17" s="21" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C17" s="21" t="s">
         <v>6</v>
       </c>
       <c r="D17" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E17" s="21" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F17" s="13">
         <f>IFERROR(VLOOKUP(B17, [1]Visited!$B$2:$C$743, 2, FALSE), "")</f>
@@ -26597,19 +26597,19 @@
     </row>
     <row r="18" spans="1:12" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A18" s="17" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B18" s="15" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C18" s="15" t="s">
         <v>6</v>
       </c>
       <c r="D18" s="15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E18" s="18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F18" s="13" t="str">
         <f>IFERROR(VLOOKUP(B18, [1]Visited!$B$2:$C$743, 2, FALSE), "")</f>

</xml_diff>